<commit_message>
Setup for month year basis
</commit_message>
<xml_diff>
--- a/CInt.xlsx
+++ b/CInt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\SM Web Development\CInterest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencermortenson/Documents/WebDev/AFM/CInterestPlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA1BF9AB-487B-41EE-839F-8DB86D87F32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF42702-43F0-A240-9C08-2756C0D25311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{67B7C52B-75BE-4750-995C-9B118151DCE0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20400" activeTab="1" xr2:uid="{67B7C52B-75BE-4750-995C-9B118151DCE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixed" sheetId="1" r:id="rId1"/>
@@ -182,11 +182,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -197,10 +198,12 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -518,13 +521,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +535,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -540,7 +543,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -548,7 +551,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -556,7 +559,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -564,7 +567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -575,17 +578,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1">
         <f ca="1">TODAY()</f>
-        <v>44645</v>
+        <v>44646</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -600,20 +603,20 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -621,7 +624,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -629,7 +632,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -640,15 +643,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -656,78 +659,78 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>46468</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1">
         <f ca="1">TODAY()</f>
-        <v>44645</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44646</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2">
         <f ca="1">(Date-B7)/365</f>
-        <v>4.9945205479452053</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2">
         <f ca="1">B8*2</f>
-        <v>9.9890410958904106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="2">
         <f ca="1">B8*4</f>
-        <v>19.978082191780821</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2">
         <f ca="1">12*B8</f>
-        <v>59.934246575342463</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="2">
         <f ca="1">B8*52</f>
-        <v>259.71506849315068</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="2">
         <f ca="1">ROUNDDOWN(B8*CF,0)</f>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -736,25 +739,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
       <c r="B16">
         <f>R_/CompF</f>
-        <v>8.3333333333333332E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="3">
         <f ca="1">((B16)*(Goal-Initial*(1+(B16))^(B13*(1/B15))))/(((1+(B16))^(B13*(1/B15))-1))/B15</f>
-        <v>24.291729217826283</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>398.46849379245265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -780,7 +783,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>0</v>
       </c>
@@ -813,334 +816,334 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>1</v>
       </c>
       <c r="B21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>5291.5007506139154</v>
+        <v>9781.6219255094329</v>
       </c>
       <c r="C21" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>291.50075061391539</v>
+        <v>4781.621925509432</v>
       </c>
       <c r="D21" s="5">
         <f t="shared" si="2"/>
-        <v>1.1047130674412968</v>
+        <v>1.0304159569135067</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="3"/>
-        <v>5523.5653372064844</v>
+        <v>5152.0797845675334</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" ref="F21:F30" ca="1" si="4">$B$17*$B$15*(D21-1)/($B$16)</f>
-        <v>305.2393775822357</v>
+        <v>4847.9202154324666</v>
       </c>
       <c r="G21" s="5">
-        <f t="shared" ref="G21:G30" ca="1" si="5">E21+F21-B21-C21</f>
-        <v>245.80321356088922</v>
+        <f ca="1">E21+F21-B21</f>
+        <v>218.37807449056709</v>
       </c>
       <c r="H21" s="5">
-        <f t="shared" ref="H21:H30" ca="1" si="6">E21+F21</f>
-        <v>5828.80471478872</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H21:H30" ca="1" si="5">E21+F21</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>2</v>
       </c>
       <c r="B22" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>5583.0015012278309</v>
+        <v>14563.243851018864</v>
       </c>
       <c r="C22" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>583.00150122783077</v>
+        <v>9563.243851018864</v>
       </c>
       <c r="D22" s="5">
         <f t="shared" si="2"/>
-        <v>1.220390961375559</v>
+        <v>1.0617570442619777</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="3"/>
-        <v>6101.9548068777949</v>
+        <v>5308.7852213098886</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>642.44130669497895</v>
+        <v>9843.2945632576339</v>
       </c>
       <c r="G22" s="5">
+        <f t="shared" ref="G22:G30" ca="1" si="6">E22+F22-B22</f>
+        <v>588.83593354865843</v>
+      </c>
+      <c r="H22" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>578.39311111711243</v>
-      </c>
-      <c r="H22" s="5">
-        <f t="shared" ca="1" si="6"/>
-        <v>6744.3961135727741</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15152.079784567522</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>3</v>
       </c>
       <c r="B23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>5874.5022518417463</v>
+        <v>19344.865776528295</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>874.5022518417461</v>
+        <v>14344.865776528295</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="2"/>
-        <v>1.3481818424188268</v>
+        <v>1.0940514007728626</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" si="3"/>
-        <v>6740.9092120941341</v>
+        <v>5470.2570038643125</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>1014.9526841522401</v>
+        <v>14990.608002013143</v>
       </c>
       <c r="G23" s="5">
+        <f t="shared" ca="1" si="6"/>
+        <v>1115.9992293491596</v>
+      </c>
+      <c r="H23" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>1006.8573925628818</v>
-      </c>
-      <c r="H23" s="5">
-        <f t="shared" ca="1" si="6"/>
-        <v>7755.8618962463743</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20460.865005877455</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>4</v>
       </c>
       <c r="B24" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>6166.0030024556618</v>
+        <v>24126.487702037728</v>
       </c>
       <c r="C24" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>1166.0030024556615</v>
+        <v>19126.487702037728</v>
       </c>
       <c r="D24" s="5">
         <f t="shared" si="2"/>
-        <v>1.4893540986071612</v>
+        <v>1.1273280210399317</v>
       </c>
       <c r="E24" s="5">
         <f t="shared" si="3"/>
-        <v>7446.7704930358059</v>
+        <v>5636.6401051996581</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>1426.4708705998346</v>
+        <v>20294.481904542117</v>
       </c>
       <c r="G24" s="5">
+        <f t="shared" ca="1" si="6"/>
+        <v>1804.6343077040474</v>
+      </c>
+      <c r="H24" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>1541.2353587243163</v>
-      </c>
-      <c r="H24" s="5">
-        <f t="shared" ca="1" si="6"/>
-        <v>8873.2413636356396</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25931.122009741775</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>5</v>
       </c>
       <c r="B25" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>6457.5037530695772</v>
+        <v>28908.109627547161</v>
       </c>
       <c r="C25" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>1457.503753069577</v>
+        <v>23908.109627547161</v>
       </c>
       <c r="D25" s="5">
         <f t="shared" si="2"/>
-        <v>1.6453089347785848</v>
+        <v>1.1616167815552709</v>
       </c>
       <c r="E25" s="5">
         <f t="shared" si="3"/>
-        <v>8226.544673892924</v>
+        <v>5808.0839077763549</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>1881.0803886582362</v>
+        <v>25759.678207165056</v>
       </c>
       <c r="G25" s="5">
+        <f t="shared" ca="1" si="6"/>
+        <v>2659.6524873942508</v>
+      </c>
+      <c r="H25" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>2192.6175564120058</v>
-      </c>
-      <c r="H25" s="5">
-        <f t="shared" ca="1" si="6"/>
-        <v>10107.62506255116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31567.762114941412</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>6</v>
       </c>
       <c r="B26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>6749.0045036834927</v>
+        <v>33689.73155305659</v>
       </c>
       <c r="C26" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>1749.0045036834922</v>
+        <v>28689.73155305659</v>
       </c>
       <c r="D26" s="5">
         <f t="shared" si="2"/>
-        <v>1.8175942802278227</v>
+        <v>1.1969484675330624</v>
       </c>
       <c r="E26" s="5">
         <f t="shared" si="3"/>
-        <v>9087.9714011391134</v>
+        <v>5984.7423376653123</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>2383.2934638405418</v>
+        <v>31391.103685052451</v>
       </c>
       <c r="G26" s="5">
+        <f t="shared" ca="1" si="6"/>
+        <v>3686.1144696611736</v>
+      </c>
+      <c r="H26" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>2973.2558576126708</v>
-      </c>
-      <c r="H26" s="5">
-        <f t="shared" ca="1" si="6"/>
-        <v>11471.264864979656</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37375.846022717764</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>7</v>
       </c>
       <c r="B27" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>7040.5052542974081</v>
+        <v>38471.353478566023</v>
       </c>
       <c r="C27" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2040.5052542974076</v>
+        <v>33471.353478566023</v>
       </c>
       <c r="D27" s="5">
         <f t="shared" si="2"/>
-        <v>2.0079201526742336</v>
+        <v>1.2333548005492361</v>
       </c>
       <c r="E27" s="5">
         <f t="shared" si="3"/>
-        <v>10039.600763371169</v>
+        <v>6166.7740027461805</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>2938.094810634313</v>
+        <v>37193.814357636918</v>
       </c>
       <c r="G27" s="5">
+        <f t="shared" ca="1" si="6"/>
+        <v>4889.2348818170794</v>
+      </c>
+      <c r="H27" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>3896.6850654106661</v>
-      </c>
-      <c r="H27" s="5">
-        <f t="shared" ca="1" si="6"/>
-        <v>12977.695574005482</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43360.588360383103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>8</v>
       </c>
       <c r="B28" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>7332.0060049113235</v>
+        <v>43252.975404075456</v>
       </c>
       <c r="C28" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2332.0060049113231</v>
+        <v>38252.975404075456</v>
       </c>
       <c r="D28" s="5">
         <f t="shared" si="2"/>
-        <v>2.2181756310379499</v>
+        <v>1.2708684670218084</v>
       </c>
       <c r="E28" s="5">
         <f t="shared" si="3"/>
-        <v>11090.87815518975</v>
+        <v>6354.3423351090423</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>3550.9911082714243</v>
+        <v>43173.020028020255</v>
       </c>
       <c r="G28" s="5">
+        <f t="shared" ca="1" si="6"/>
+        <v>6274.3869590538452</v>
+      </c>
+      <c r="H28" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>4977.8572536385273</v>
-      </c>
-      <c r="H28" s="5">
-        <f t="shared" ca="1" si="6"/>
-        <v>14641.869263461174</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>49527.362363129301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>9</v>
       </c>
       <c r="B29" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>7623.506755525239</v>
+        <v>48034.597329584889</v>
       </c>
       <c r="C29" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2623.5067555252385</v>
+        <v>43034.597329584889</v>
       </c>
       <c r="D29" s="5">
         <f t="shared" si="2"/>
-        <v>2.4504476054874678</v>
+        <v>1.309523147557478</v>
       </c>
       <c r="E29" s="5">
         <f t="shared" si="3"/>
-        <v>12252.238027437339</v>
+        <v>6547.6157377873897</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>4228.0656572575317</v>
+        <v>49334.088960450928</v>
       </c>
       <c r="G29" s="5">
+        <f t="shared" ca="1" si="6"/>
+        <v>7847.1073686534291</v>
+      </c>
+      <c r="H29" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>6233.2901736443928</v>
-      </c>
-      <c r="H29" s="5">
-        <f t="shared" ca="1" si="6"/>
-        <v>16480.303684694871</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>55881.704698238318</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>10</v>
       </c>
       <c r="B30" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>7915.0075061391544</v>
+        <v>52816.219255094322</v>
       </c>
       <c r="C30" s="5">
         <f t="shared" ca="1" si="1"/>
-        <v>2915.007506139154</v>
+        <v>47816.219255094322</v>
       </c>
       <c r="D30" s="5">
         <f t="shared" si="2"/>
-        <v>2.7070414908622409</v>
+        <v>1.3493535471908258</v>
       </c>
       <c r="E30" s="5">
         <f t="shared" si="3"/>
-        <v>13535.207454311205</v>
+        <v>6746.7677359541285</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>4976.038759154404</v>
+        <v>55682.552700071552</v>
       </c>
       <c r="G30" s="5">
+        <f t="shared" ca="1" si="6"/>
+        <v>9613.1011809313568</v>
+      </c>
+      <c r="H30" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>7681.2312011873</v>
-      </c>
-      <c r="H30" s="5">
-        <f t="shared" ca="1" si="6"/>
-        <v>18511.246213465609</v>
+        <v>62429.320436025679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>